<commit_message>
CIERRE 28 OCT 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #10  OCTUBRE 2022/BALANCE   HERRADURA  OCTUBRE      2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #10  OCTUBRE 2022/BALANCE   HERRADURA  OCTUBRE      2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="195" yWindow="915" windowWidth="16905" windowHeight="10110" firstSheet="18" activeTab="18"/>
+    <workbookView xWindow="195" yWindow="915" windowWidth="16905" windowHeight="10110" firstSheet="16" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 2         " sheetId="1" r:id="rId1"/>
@@ -632,7 +632,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="515">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2187,6 +2187,9 @@
   </si>
   <si>
     <t>NOMINA # 41</t>
+  </si>
+  <si>
+    <t>NOMINA # 42</t>
   </si>
 </sst>
 </file>
@@ -4227,6 +4230,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="44" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4306,39 +4342,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8933,23 +8936,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -8959,21 +8962,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -8988,14 +8991,14 @@
       <c r="D4" s="16">
         <v>44563</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -9005,11 +9008,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -10464,11 +10467,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="380">
+      <c r="M40" s="391">
         <f>SUM(M5:M39)</f>
         <v>1527030</v>
       </c>
-      <c r="N40" s="382">
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
         <v>50013</v>
       </c>
@@ -10493,8 +10496,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="74"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -10701,29 +10704,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="384" t="s">
+      <c r="H53" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="385"/>
+      <c r="I53" s="396"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="386">
+      <c r="K53" s="397">
         <f>I51+L51</f>
         <v>50143.28</v>
       </c>
-      <c r="L53" s="387"/>
-      <c r="M53" s="388">
+      <c r="L53" s="398"/>
+      <c r="M53" s="399">
         <f>N40+M40</f>
         <v>1577043</v>
       </c>
-      <c r="N53" s="389"/>
+      <c r="N53" s="400"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="390" t="s">
+      <c r="D54" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="390"/>
+      <c r="E54" s="401"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>1561421.72</v>
@@ -10734,22 +10737,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="391" t="s">
+      <c r="D55" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="391"/>
+      <c r="E55" s="402"/>
       <c r="F55" s="111">
         <v>-1419082.77</v>
       </c>
-      <c r="I55" s="392" t="s">
+      <c r="I55" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="393"/>
-      <c r="K55" s="394">
+      <c r="J55" s="404"/>
+      <c r="K55" s="405">
         <f>F57+F58+F59</f>
         <v>296963.46999999997</v>
       </c>
-      <c r="L55" s="395"/>
+      <c r="L55" s="406"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -10780,11 +10783,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="396">
+      <c r="K57" s="407">
         <f>-C4</f>
         <v>-221059.7</v>
       </c>
-      <c r="L57" s="397"/>
+      <c r="L57" s="408"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -10801,22 +10804,22 @@
       <c r="C59" s="128">
         <v>44591</v>
       </c>
-      <c r="D59" s="373" t="s">
+      <c r="D59" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="374"/>
+      <c r="E59" s="385"/>
       <c r="F59" s="129">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="375" t="s">
+      <c r="I59" s="386" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="376"/>
-      <c r="K59" s="377">
+      <c r="J59" s="387"/>
+      <c r="K59" s="388">
         <f>K55+K57</f>
         <v>75903.76999999996</v>
       </c>
-      <c r="L59" s="377"/>
+      <c r="L59" s="388"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -10941,12 +10944,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
@@ -10962,6 +10959,12 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12414,23 +12417,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -12440,21 +12443,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -12469,14 +12472,14 @@
       <c r="D4" s="16">
         <v>44710</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -12486,11 +12489,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -14020,11 +14023,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="380">
+      <c r="M40" s="391">
         <f>SUM(M5:M39)</f>
         <v>2772689</v>
       </c>
-      <c r="N40" s="382">
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
         <v>107354</v>
       </c>
@@ -14055,8 +14058,8 @@
       <c r="L41" s="73">
         <v>638.99</v>
       </c>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -14302,29 +14305,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="384" t="s">
+      <c r="H53" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="385"/>
+      <c r="I53" s="396"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="386">
+      <c r="K53" s="397">
         <f>I51+L51</f>
         <v>60691.69</v>
       </c>
-      <c r="L53" s="387"/>
-      <c r="M53" s="388">
+      <c r="L53" s="398"/>
+      <c r="M53" s="399">
         <f>N40+M40</f>
         <v>2880043</v>
       </c>
-      <c r="N53" s="389"/>
+      <c r="N53" s="400"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="390" t="s">
+      <c r="D54" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="390"/>
+      <c r="E54" s="401"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2844548.31</v>
@@ -14335,22 +14338,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="391" t="s">
+      <c r="D55" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="391"/>
+      <c r="E55" s="402"/>
       <c r="F55" s="111">
         <v>-2875380.48</v>
       </c>
-      <c r="I55" s="392" t="s">
+      <c r="I55" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="393"/>
-      <c r="K55" s="394">
+      <c r="J55" s="404"/>
+      <c r="K55" s="405">
         <f>F57+F58+F59</f>
         <v>247554.74000000008</v>
       </c>
-      <c r="L55" s="395"/>
+      <c r="L55" s="406"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -14381,11 +14384,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="396">
+      <c r="K57" s="407">
         <f>-C4</f>
         <v>-149938.81</v>
       </c>
-      <c r="L57" s="397"/>
+      <c r="L57" s="408"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -14402,22 +14405,22 @@
       <c r="C59" s="128">
         <v>44745</v>
       </c>
-      <c r="D59" s="373" t="s">
+      <c r="D59" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="374"/>
+      <c r="E59" s="385"/>
       <c r="F59" s="129">
         <v>232165.91</v>
       </c>
-      <c r="I59" s="375" t="s">
+      <c r="I59" s="386" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="376"/>
-      <c r="K59" s="377">
+      <c r="J59" s="387"/>
+      <c r="K59" s="388">
         <f>K55+K57</f>
         <v>97615.93000000008</v>
       </c>
-      <c r="L59" s="377"/>
+      <c r="L59" s="388"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -14545,6 +14548,18 @@
     <sortCondition ref="B7:B9"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -14554,18 +14569,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.38" right="0.17" top="0.4" bottom="0.34" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -16047,23 +16050,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -16073,21 +16076,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -16102,14 +16105,14 @@
       <c r="D4" s="16">
         <v>44745</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -16119,11 +16122,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -17568,11 +17571,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="380">
+      <c r="M40" s="391">
         <f>SUM(M5:M39)</f>
         <v>2373103</v>
       </c>
-      <c r="N40" s="382">
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
         <v>67308</v>
       </c>
@@ -17601,8 +17604,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -17817,29 +17820,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="384" t="s">
+      <c r="H53" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="385"/>
+      <c r="I53" s="396"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="386">
+      <c r="K53" s="397">
         <f>I51+L51</f>
         <v>79649.720000000016</v>
       </c>
-      <c r="L53" s="387"/>
-      <c r="M53" s="388">
+      <c r="L53" s="398"/>
+      <c r="M53" s="399">
         <f>N40+M40</f>
         <v>2440411</v>
       </c>
-      <c r="N53" s="389"/>
+      <c r="N53" s="400"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="390" t="s">
+      <c r="D54" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="390"/>
+      <c r="E54" s="401"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2356249.2799999998</v>
@@ -17850,22 +17853,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="391" t="s">
+      <c r="D55" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="391"/>
+      <c r="E55" s="402"/>
       <c r="F55" s="111">
         <v>-2471332.31</v>
       </c>
-      <c r="I55" s="392" t="s">
+      <c r="I55" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="393"/>
-      <c r="K55" s="394">
+      <c r="J55" s="404"/>
+      <c r="K55" s="405">
         <f>F57+F58+F59</f>
         <v>214026.38999999972</v>
       </c>
-      <c r="L55" s="395"/>
+      <c r="L55" s="406"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -17896,11 +17899,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="396">
+      <c r="K57" s="407">
         <f>-C4</f>
         <v>-232165.91</v>
       </c>
-      <c r="L57" s="397"/>
+      <c r="L57" s="408"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -17917,22 +17920,22 @@
       <c r="C59" s="128">
         <v>44773</v>
       </c>
-      <c r="D59" s="373" t="s">
+      <c r="D59" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="374"/>
+      <c r="E59" s="385"/>
       <c r="F59" s="129">
         <v>273736.42</v>
       </c>
-      <c r="I59" s="375" t="s">
+      <c r="I59" s="386" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="376"/>
-      <c r="K59" s="377">
+      <c r="J59" s="387"/>
+      <c r="K59" s="388">
         <f>K55+K57</f>
         <v>-18139.520000000281</v>
       </c>
-      <c r="L59" s="377"/>
+      <c r="L59" s="388"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -18057,6 +18060,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -18066,18 +18081,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.27559055118110237" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="60" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19469,23 +19472,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>421</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -19495,21 +19498,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -19524,14 +19527,14 @@
       <c r="D4" s="16">
         <v>44773</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -19541,11 +19544,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -21025,11 +21028,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="380">
+      <c r="M40" s="391">
         <f>SUM(M5:M39)</f>
         <v>2375259</v>
       </c>
-      <c r="N40" s="382">
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
         <v>61117</v>
       </c>
@@ -21058,8 +21061,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -21274,29 +21277,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="384" t="s">
+      <c r="H53" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="385"/>
+      <c r="I53" s="396"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="386">
+      <c r="K53" s="397">
         <f>I51+L51</f>
         <v>52857.25</v>
       </c>
-      <c r="L53" s="387"/>
-      <c r="M53" s="388">
+      <c r="L53" s="398"/>
+      <c r="M53" s="399">
         <f>N40+M40</f>
         <v>2436376</v>
       </c>
-      <c r="N53" s="389"/>
+      <c r="N53" s="400"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="390" t="s">
+      <c r="D54" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="390"/>
+      <c r="E54" s="401"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2370653.75</v>
@@ -21307,22 +21310,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="391" t="s">
+      <c r="D55" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="391"/>
+      <c r="E55" s="402"/>
       <c r="F55" s="111">
         <v>-2401197.5699999998</v>
       </c>
-      <c r="I55" s="392" t="s">
+      <c r="I55" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="393"/>
-      <c r="K55" s="394">
+      <c r="J55" s="404"/>
+      <c r="K55" s="405">
         <f>F57+F58+F59</f>
         <v>259241.77000000016</v>
       </c>
-      <c r="L55" s="395"/>
+      <c r="L55" s="406"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -21353,11 +21356,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="396">
+      <c r="K57" s="407">
         <f>-C4</f>
         <v>-273736.42</v>
       </c>
-      <c r="L57" s="397"/>
+      <c r="L57" s="408"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -21374,10 +21377,10 @@
       <c r="C59" s="128">
         <v>44801</v>
       </c>
-      <c r="D59" s="373" t="s">
+      <c r="D59" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="374"/>
+      <c r="E59" s="385"/>
       <c r="F59" s="129">
         <v>236400.59</v>
       </c>
@@ -21514,6 +21517,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -21523,18 +21538,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22913,10 +22916,10 @@
   <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22941,23 +22944,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>465</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -22967,21 +22970,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -22996,14 +22999,14 @@
       <c r="D4" s="16">
         <v>44801</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -23013,11 +23016,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -24745,11 +24748,11 @@
       <c r="L40" s="73">
         <v>927.48</v>
       </c>
-      <c r="M40" s="380">
+      <c r="M40" s="391">
         <f>SUM(M5:M39)</f>
         <v>3147309.5</v>
       </c>
-      <c r="N40" s="382">
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
         <v>76569</v>
       </c>
@@ -24784,8 +24787,8 @@
       <c r="L41" s="73">
         <v>33312</v>
       </c>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -25028,29 +25031,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="384" t="s">
+      <c r="H53" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="385"/>
+      <c r="I53" s="396"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="386">
+      <c r="K53" s="397">
         <f>I51+L51</f>
         <v>102873.87000000001</v>
       </c>
-      <c r="L53" s="387"/>
-      <c r="M53" s="388">
+      <c r="L53" s="398"/>
+      <c r="M53" s="399">
         <f>N40+M40</f>
         <v>3223878.5</v>
       </c>
-      <c r="N53" s="389"/>
+      <c r="N53" s="400"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="390" t="s">
+      <c r="D54" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="390"/>
+      <c r="E54" s="401"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>3130076.13</v>
@@ -25061,22 +25064,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="391" t="s">
+      <c r="D55" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="391"/>
+      <c r="E55" s="402"/>
       <c r="F55" s="111">
         <v>-3171951.31</v>
       </c>
-      <c r="I55" s="392" t="s">
+      <c r="I55" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="393"/>
-      <c r="K55" s="394">
+      <c r="J55" s="404"/>
+      <c r="K55" s="405">
         <f>F57+F58+F59</f>
         <v>265314.0299999998</v>
       </c>
-      <c r="L55" s="395"/>
+      <c r="L55" s="406"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -25107,11 +25110,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="396">
+      <c r="K57" s="407">
         <f>-C4</f>
         <v>-236400.59</v>
       </c>
-      <c r="L57" s="397"/>
+      <c r="L57" s="408"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -25128,10 +25131,10 @@
       <c r="C59" s="128">
         <v>44836</v>
       </c>
-      <c r="D59" s="373" t="s">
+      <c r="D59" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="374"/>
+      <c r="E59" s="385"/>
       <c r="F59" s="129">
         <v>242354.21</v>
       </c>
@@ -25271,18 +25274,6 @@
     <sortCondition ref="J41:J45"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -25292,6 +25283,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -26608,10 +26611,10 @@
   <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
+      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26636,23 +26639,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>512</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -26662,21 +26665,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -26691,14 +26694,14 @@
       <c r="D4" s="16">
         <v>44836</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -26708,11 +26711,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -27175,25 +27178,29 @@
       <c r="E14" s="322">
         <v>44846</v>
       </c>
-      <c r="F14" s="27"/>
+      <c r="F14" s="27">
+        <v>57382</v>
+      </c>
       <c r="G14" s="323"/>
       <c r="H14" s="324">
         <v>44846</v>
       </c>
-      <c r="I14" s="29"/>
+      <c r="I14" s="29">
+        <v>166</v>
+      </c>
       <c r="J14" s="36"/>
       <c r="K14" s="330"/>
       <c r="L14" s="38"/>
       <c r="M14" s="30">
-        <v>0</v>
+        <v>56283</v>
       </c>
       <c r="N14" s="31">
-        <v>0</v>
+        <v>933</v>
       </c>
       <c r="O14" s="314"/>
       <c r="P14" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>57382</v>
       </c>
       <c r="Q14" s="12">
         <f t="shared" si="0"/>
@@ -27212,23 +27219,30 @@
         <v>44847</v>
       </c>
       <c r="C15" s="24">
-        <v>0</v>
-      </c>
-      <c r="D15" s="335"/>
+        <v>20305.2</v>
+      </c>
+      <c r="D15" s="335" t="s">
+        <v>49</v>
+      </c>
       <c r="E15" s="322">
         <v>44847</v>
       </c>
-      <c r="F15" s="27"/>
+      <c r="F15" s="27">
+        <v>98367</v>
+      </c>
       <c r="G15" s="323"/>
       <c r="H15" s="324">
         <v>44847</v>
       </c>
-      <c r="I15" s="29"/>
+      <c r="I15" s="29">
+        <v>125</v>
+      </c>
       <c r="J15" s="36"/>
       <c r="K15" s="330"/>
       <c r="L15" s="38"/>
       <c r="M15" s="30">
-        <v>0</v>
+        <f>20000+57937</f>
+        <v>77937</v>
       </c>
       <c r="N15" s="31">
         <v>0</v>
@@ -27236,11 +27250,11 @@
       <c r="O15" s="314"/>
       <c r="P15" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>98367.2</v>
       </c>
       <c r="Q15" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.19999999999708962</v>
       </c>
       <c r="R15" s="12">
         <v>0</v>
@@ -27255,23 +27269,30 @@
         <v>44848</v>
       </c>
       <c r="C16" s="24">
-        <v>0</v>
-      </c>
-      <c r="D16" s="326"/>
+        <v>4395</v>
+      </c>
+      <c r="D16" s="326" t="s">
+        <v>279</v>
+      </c>
       <c r="E16" s="322">
         <v>44848</v>
       </c>
-      <c r="F16" s="27"/>
+      <c r="F16" s="27">
+        <v>124865</v>
+      </c>
       <c r="G16" s="323"/>
       <c r="H16" s="324">
         <v>44848</v>
       </c>
-      <c r="I16" s="29"/>
+      <c r="I16" s="29">
+        <v>334</v>
+      </c>
       <c r="J16" s="36"/>
       <c r="K16" s="330"/>
       <c r="L16" s="8"/>
       <c r="M16" s="30">
-        <v>0</v>
+        <f>70136+50000</f>
+        <v>120136</v>
       </c>
       <c r="N16" s="31">
         <v>0</v>
@@ -27279,7 +27300,7 @@
       <c r="O16" s="314"/>
       <c r="P16" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>124865</v>
       </c>
       <c r="Q16" s="12">
         <f t="shared" si="0"/>
@@ -27304,32 +27325,42 @@
       <c r="E17" s="322">
         <v>44849</v>
       </c>
-      <c r="F17" s="27"/>
+      <c r="F17" s="27">
+        <v>126961</v>
+      </c>
       <c r="G17" s="323"/>
       <c r="H17" s="324">
         <v>44849</v>
       </c>
-      <c r="I17" s="29"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="336"/>
-      <c r="L17" s="46"/>
+      <c r="I17" s="29">
+        <v>155</v>
+      </c>
+      <c r="J17" s="36">
+        <v>44849</v>
+      </c>
+      <c r="K17" s="336" t="s">
+        <v>514</v>
+      </c>
+      <c r="L17" s="46">
+        <v>9500</v>
+      </c>
       <c r="M17" s="30">
-        <v>0</v>
+        <f>60000+49530</f>
+        <v>109530</v>
       </c>
       <c r="N17" s="31">
-        <v>0</v>
+        <v>8836</v>
       </c>
       <c r="O17" s="314"/>
       <c r="P17" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>128021</v>
       </c>
       <c r="Q17" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="8">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="R17" s="176">
+        <v>1060</v>
       </c>
       <c r="S17" s="369">
         <v>44849</v>
@@ -27341,31 +27372,38 @@
         <v>44850</v>
       </c>
       <c r="C18" s="24">
-        <v>0</v>
-      </c>
-      <c r="D18" s="326"/>
+        <v>480</v>
+      </c>
+      <c r="D18" s="326" t="s">
+        <v>47</v>
+      </c>
       <c r="E18" s="322">
         <v>44850</v>
       </c>
-      <c r="F18" s="27"/>
+      <c r="F18" s="27">
+        <v>132540</v>
+      </c>
       <c r="G18" s="323"/>
       <c r="H18" s="324">
         <v>44850</v>
       </c>
-      <c r="I18" s="29"/>
+      <c r="I18" s="29">
+        <v>80</v>
+      </c>
       <c r="J18" s="36"/>
       <c r="K18" s="337"/>
       <c r="L18" s="38"/>
       <c r="M18" s="30">
-        <v>0</v>
+        <f>75000+52964</f>
+        <v>127964</v>
       </c>
       <c r="N18" s="31">
-        <v>0</v>
+        <v>4016</v>
       </c>
       <c r="O18" s="314"/>
       <c r="P18" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>132540</v>
       </c>
       <c r="Q18" s="12">
         <f t="shared" si="0"/>
@@ -27402,9 +27440,7 @@
       <c r="M19" s="30">
         <v>0</v>
       </c>
-      <c r="N19" s="31">
-        <v>0</v>
-      </c>
+      <c r="N19" s="31"/>
       <c r="O19" s="314"/>
       <c r="P19" s="32">
         <f t="shared" si="1"/>
@@ -28224,25 +28260,25 @@
       <c r="J40" s="71"/>
       <c r="K40" s="360"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="380">
+      <c r="M40" s="391">
         <f>SUM(M5:M39)</f>
-        <v>756696</v>
-      </c>
-      <c r="N40" s="382">
+        <v>1248546</v>
+      </c>
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
-        <v>20594</v>
+        <v>34379</v>
       </c>
       <c r="P40" s="32">
         <f t="shared" si="1"/>
-        <v>777290</v>
+        <v>1282925</v>
       </c>
       <c r="Q40" s="284">
         <f>SUM(Q5:Q39)</f>
-        <v>0</v>
+        <v>0.19999999999708962</v>
       </c>
       <c r="R40" s="316">
         <f>SUM(R5:R39)</f>
-        <v>63775</v>
+        <v>64835</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -28258,8 +28294,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="363"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -28432,7 +28468,7 @@
       </c>
       <c r="C51" s="102">
         <f>SUM(C5:C50)</f>
-        <v>27773</v>
+        <v>52953.2</v>
       </c>
       <c r="D51" s="103"/>
       <c r="E51" s="104" t="s">
@@ -28440,7 +28476,7 @@
       </c>
       <c r="F51" s="105">
         <f>SUM(F5:F50)</f>
-        <v>752090</v>
+        <v>1292205</v>
       </c>
       <c r="G51" s="103"/>
       <c r="H51" s="106" t="s">
@@ -28448,7 +28484,7 @@
       </c>
       <c r="I51" s="107">
         <f>SUM(I5:I50)</f>
-        <v>907</v>
+        <v>1767</v>
       </c>
       <c r="J51" s="108"/>
       <c r="K51" s="109" t="s">
@@ -28456,7 +28492,7 @@
       </c>
       <c r="L51" s="110">
         <f>SUM(L5:L50)</f>
-        <v>9841</v>
+        <v>19341</v>
       </c>
       <c r="M51" s="111"/>
       <c r="N51" s="111"/>
@@ -28474,32 +28510,32 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="384" t="s">
+      <c r="H53" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="385"/>
+      <c r="I53" s="396"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="386">
+      <c r="K53" s="397">
         <f>I51+L51</f>
-        <v>10748</v>
-      </c>
-      <c r="L53" s="387"/>
-      <c r="M53" s="388">
+        <v>21108</v>
+      </c>
+      <c r="L53" s="398"/>
+      <c r="M53" s="399">
         <f>N40+M40</f>
-        <v>777290</v>
-      </c>
-      <c r="N53" s="389"/>
+        <v>1282925</v>
+      </c>
+      <c r="N53" s="400"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="390" t="s">
+      <c r="D54" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="390"/>
+      <c r="E54" s="401"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
-        <v>713569</v>
+        <v>1218143.8</v>
       </c>
       <c r="I54" s="116"/>
       <c r="J54" s="117"/>
@@ -28507,22 +28543,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="391" t="s">
+      <c r="D55" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="391"/>
+      <c r="E55" s="402"/>
       <c r="F55" s="111">
         <v>0</v>
       </c>
-      <c r="I55" s="392" t="s">
+      <c r="I55" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="393"/>
-      <c r="K55" s="394">
+      <c r="J55" s="404"/>
+      <c r="K55" s="405">
         <f>F57+F58+F59</f>
-        <v>713569</v>
-      </c>
-      <c r="L55" s="395"/>
+        <v>1218143.8</v>
+      </c>
+      <c r="L55" s="406"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -28546,18 +28582,18 @@
       </c>
       <c r="F57" s="111">
         <f>SUM(F54:F56)</f>
-        <v>713569</v>
+        <v>1218143.8</v>
       </c>
       <c r="H57" s="22"/>
       <c r="I57" s="124" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="396">
+      <c r="K57" s="407">
         <f>-C4</f>
         <v>-242354.21</v>
       </c>
-      <c r="L57" s="397"/>
+      <c r="L57" s="408"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -28572,10 +28608,10 @@
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="128"/>
-      <c r="D59" s="373" t="s">
+      <c r="D59" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="374"/>
+      <c r="E59" s="385"/>
       <c r="F59" s="129">
         <v>0</v>
       </c>
@@ -28585,7 +28621,7 @@
       <c r="J59" s="411"/>
       <c r="K59" s="412">
         <f>K55+K57</f>
-        <v>471214.79000000004</v>
+        <v>975789.59000000008</v>
       </c>
       <c r="L59" s="412"/>
     </row>
@@ -28712,20 +28748,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="M53:N53"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
@@ -28733,6 +28755,20 @@
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="M53:N53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31633,23 +31669,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -31659,21 +31695,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -31688,14 +31724,14 @@
       <c r="D4" s="16">
         <v>44591</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -31705,11 +31741,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -33150,7 +33186,7 @@
         <f>SUM(M5:M39)</f>
         <v>1636108</v>
       </c>
-      <c r="N40" s="382">
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
         <v>55675</v>
       </c>
@@ -33175,8 +33211,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="74"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -33383,29 +33419,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="384" t="s">
+      <c r="H53" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="385"/>
+      <c r="I53" s="396"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="386">
+      <c r="K53" s="397">
         <f>I51+L51</f>
         <v>45634.280000000006</v>
       </c>
-      <c r="L53" s="387"/>
-      <c r="M53" s="388">
+      <c r="L53" s="398"/>
+      <c r="M53" s="399">
         <f>N40+M40</f>
         <v>1691783</v>
       </c>
-      <c r="N53" s="389"/>
+      <c r="N53" s="400"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="390" t="s">
+      <c r="D54" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="390"/>
+      <c r="E54" s="401"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>1686442.72</v>
@@ -33416,22 +33452,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="391" t="s">
+      <c r="D55" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="391"/>
+      <c r="E55" s="402"/>
       <c r="F55" s="111">
         <v>-1631962.77</v>
       </c>
-      <c r="I55" s="392" t="s">
+      <c r="I55" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="393"/>
-      <c r="K55" s="394">
+      <c r="J55" s="404"/>
+      <c r="K55" s="405">
         <f>F57+F58+F59</f>
         <v>238822.13999999996</v>
       </c>
-      <c r="L55" s="395"/>
+      <c r="L55" s="406"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -33462,11 +33498,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="396">
+      <c r="K57" s="407">
         <f>-C4</f>
         <v>-154314.51999999999</v>
       </c>
-      <c r="L57" s="397"/>
+      <c r="L57" s="408"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -33483,22 +33519,22 @@
       <c r="C59" s="128">
         <v>44619</v>
       </c>
-      <c r="D59" s="373" t="s">
+      <c r="D59" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="374"/>
+      <c r="E59" s="385"/>
       <c r="F59" s="129">
         <v>184342.19</v>
       </c>
-      <c r="I59" s="375" t="s">
+      <c r="I59" s="386" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="376"/>
-      <c r="K59" s="377">
+      <c r="J59" s="387"/>
+      <c r="K59" s="388">
         <f>K55+K57</f>
         <v>84507.619999999966</v>
       </c>
-      <c r="L59" s="377"/>
+      <c r="L59" s="388"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -33623,18 +33659,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -33644,6 +33668,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -34948,23 +34984,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -34974,21 +35010,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -35003,14 +35039,14 @@
       <c r="D4" s="16">
         <v>44619</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -35020,11 +35056,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -36475,11 +36511,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="380">
+      <c r="M40" s="391">
         <f>SUM(M5:M39)</f>
         <v>1793435</v>
       </c>
-      <c r="N40" s="382">
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
         <v>63995</v>
       </c>
@@ -36504,8 +36540,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -36644,29 +36680,29 @@
       <c r="A49" s="33"/>
       <c r="B49" s="113"/>
       <c r="C49" s="1"/>
-      <c r="H49" s="384" t="s">
+      <c r="H49" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="385"/>
+      <c r="I49" s="396"/>
       <c r="J49" s="114"/>
-      <c r="K49" s="386">
+      <c r="K49" s="397">
         <f>I47+L47</f>
         <v>90434.03</v>
       </c>
-      <c r="L49" s="387"/>
-      <c r="M49" s="388">
+      <c r="L49" s="398"/>
+      <c r="M49" s="399">
         <f>N40+M40</f>
         <v>1857430</v>
       </c>
-      <c r="N49" s="389"/>
+      <c r="N49" s="400"/>
       <c r="P49" s="32"/>
       <c r="Q49" s="8"/>
     </row>
     <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D50" s="390" t="s">
+      <c r="D50" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="390"/>
+      <c r="E50" s="401"/>
       <c r="F50" s="115">
         <f>F47-K49-C47</f>
         <v>1824260.97</v>
@@ -36677,22 +36713,22 @@
       <c r="Q50" s="8"/>
     </row>
     <row r="51" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D51" s="391" t="s">
+      <c r="D51" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="391"/>
+      <c r="E51" s="402"/>
       <c r="F51" s="111">
         <v>-1848136.64</v>
       </c>
-      <c r="I51" s="392" t="s">
+      <c r="I51" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J51" s="393"/>
-      <c r="K51" s="394">
+      <c r="J51" s="404"/>
+      <c r="K51" s="405">
         <f>F53+F54+F55</f>
         <v>195541.70000000007</v>
       </c>
-      <c r="L51" s="395"/>
+      <c r="L51" s="406"/>
       <c r="P51" s="32"/>
       <c r="Q51" s="8"/>
     </row>
@@ -36723,11 +36759,11 @@
         <v>17</v>
       </c>
       <c r="J53" s="125"/>
-      <c r="K53" s="396">
+      <c r="K53" s="407">
         <f>-C4</f>
         <v>-184342.19</v>
       </c>
-      <c r="L53" s="397"/>
+      <c r="L53" s="408"/>
     </row>
     <row r="54" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="126" t="s">
@@ -36744,22 +36780,22 @@
       <c r="C55" s="128">
         <v>44647</v>
       </c>
-      <c r="D55" s="373" t="s">
+      <c r="D55" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="374"/>
+      <c r="E55" s="385"/>
       <c r="F55" s="129">
         <v>219417.37</v>
       </c>
-      <c r="I55" s="375" t="s">
+      <c r="I55" s="386" t="s">
         <v>226</v>
       </c>
-      <c r="J55" s="376"/>
-      <c r="K55" s="377">
+      <c r="J55" s="387"/>
+      <c r="K55" s="388">
         <f>K51+K53</f>
         <v>11199.510000000068</v>
       </c>
-      <c r="L55" s="377"/>
+      <c r="L55" s="388"/>
     </row>
     <row r="56" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C56" s="130"/>
@@ -36887,6 +36923,18 @@
     <sortCondition ref="J34:J38"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -36896,18 +36944,6 @@
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="K49:L49"/>
     <mergeCell ref="M49:N49"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -38382,23 +38418,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -38408,21 +38444,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -38437,14 +38473,14 @@
       <c r="D4" s="16">
         <v>44647</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -38454,11 +38490,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -40055,11 +40091,11 @@
         <f>927.48+128</f>
         <v>1055.48</v>
       </c>
-      <c r="M40" s="380">
+      <c r="M40" s="391">
         <f>SUM(M5:M39)</f>
         <v>2146671</v>
       </c>
-      <c r="N40" s="382">
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
         <v>68590</v>
       </c>
@@ -40090,8 +40126,8 @@
       <c r="L41" s="73">
         <v>1195.68</v>
       </c>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -40322,29 +40358,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="384" t="s">
+      <c r="H53" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="385"/>
+      <c r="I53" s="396"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="386">
+      <c r="K53" s="397">
         <f>I51+L51</f>
         <v>91272.77</v>
       </c>
-      <c r="L53" s="387"/>
-      <c r="M53" s="388">
+      <c r="L53" s="398"/>
+      <c r="M53" s="399">
         <f>N40+M40</f>
         <v>2215261</v>
       </c>
-      <c r="N53" s="389"/>
+      <c r="N53" s="400"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="390" t="s">
+      <c r="D54" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="390"/>
+      <c r="E54" s="401"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2179879.23</v>
@@ -40355,22 +40391,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="391" t="s">
+      <c r="D55" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="391"/>
+      <c r="E55" s="402"/>
       <c r="F55" s="111">
         <v>-2227493.48</v>
       </c>
-      <c r="I55" s="392" t="s">
+      <c r="I55" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="393"/>
-      <c r="K55" s="394">
+      <c r="J55" s="404"/>
+      <c r="K55" s="405">
         <f>F57+F58+F59</f>
         <v>261521.34000000003</v>
       </c>
-      <c r="L55" s="395"/>
+      <c r="L55" s="406"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -40401,11 +40437,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="396">
+      <c r="K57" s="407">
         <f>-C4</f>
         <v>-219417.37</v>
       </c>
-      <c r="L57" s="397"/>
+      <c r="L57" s="408"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -40422,22 +40458,22 @@
       <c r="C59" s="128">
         <v>44682</v>
       </c>
-      <c r="D59" s="373" t="s">
+      <c r="D59" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="374"/>
+      <c r="E59" s="385"/>
       <c r="F59" s="129">
         <v>297874.59000000003</v>
       </c>
-      <c r="I59" s="375" t="s">
+      <c r="I59" s="386" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="376"/>
-      <c r="K59" s="377">
+      <c r="J59" s="387"/>
+      <c r="K59" s="388">
         <f>K55+K57</f>
         <v>42103.97000000003</v>
       </c>
-      <c r="L59" s="377"/>
+      <c r="L59" s="388"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -40565,6 +40601,18 @@
     <sortCondition ref="J40:J44"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -40574,18 +40622,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -42089,23 +42125,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="398"/>
-      <c r="C1" s="400" t="s">
+      <c r="B1" s="371"/>
+      <c r="C1" s="373" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="401"/>
-      <c r="I1" s="401"/>
-      <c r="J1" s="401"/>
-      <c r="K1" s="401"/>
-      <c r="L1" s="401"/>
-      <c r="M1" s="401"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
+      <c r="I1" s="374"/>
+      <c r="J1" s="374"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
+      <c r="M1" s="374"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="399"/>
+      <c r="B2" s="372"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -42115,21 +42151,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="402" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="403"/>
+      <c r="B3" s="375" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="376"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="404" t="s">
+      <c r="H3" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="404"/>
+      <c r="I3" s="377"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="371" t="s">
+      <c r="R3" s="382" t="s">
         <v>38</v>
       </c>
     </row>
@@ -42144,14 +42180,14 @@
       <c r="D4" s="16">
         <v>44682</v>
       </c>
-      <c r="E4" s="405" t="s">
+      <c r="E4" s="378" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="406"/>
-      <c r="H4" s="407" t="s">
+      <c r="F4" s="379"/>
+      <c r="H4" s="380" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="408"/>
+      <c r="I4" s="381"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -42161,11 +42197,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="378" t="s">
+      <c r="P4" s="389" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="372"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="383"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -43682,11 +43718,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="380">
+      <c r="M40" s="391">
         <f>SUM(M5:M39)</f>
         <v>2144215</v>
       </c>
-      <c r="N40" s="382">
+      <c r="N40" s="393">
         <f>SUM(N5:N39)</f>
         <v>62525</v>
       </c>
@@ -43711,8 +43747,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="381"/>
-      <c r="N41" s="383"/>
+      <c r="M41" s="392"/>
+      <c r="N41" s="394"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -43923,29 +43959,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="384" t="s">
+      <c r="H53" s="395" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="385"/>
+      <c r="I53" s="396"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="386">
+      <c r="K53" s="397">
         <f>I51+L51</f>
         <v>51231.42</v>
       </c>
-      <c r="L53" s="387"/>
-      <c r="M53" s="388">
+      <c r="L53" s="398"/>
+      <c r="M53" s="399">
         <f>N40+M40</f>
         <v>2206740</v>
       </c>
-      <c r="N53" s="389"/>
+      <c r="N53" s="400"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="390" t="s">
+      <c r="D54" s="401" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="390"/>
+      <c r="E54" s="401"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2189405.58</v>
@@ -43956,22 +43992,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="391" t="s">
+      <c r="D55" s="402" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="391"/>
+      <c r="E55" s="402"/>
       <c r="F55" s="111">
         <v>-2251924.65</v>
       </c>
-      <c r="I55" s="392" t="s">
+      <c r="I55" s="403" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="393"/>
-      <c r="K55" s="394">
+      <c r="J55" s="404"/>
+      <c r="K55" s="405">
         <f>F57+F58+F59</f>
         <v>112552.74000000017</v>
       </c>
-      <c r="L55" s="395"/>
+      <c r="L55" s="406"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -44002,11 +44038,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="396">
+      <c r="K57" s="407">
         <f>-C4</f>
         <v>-297874.59000000003</v>
       </c>
-      <c r="L57" s="397"/>
+      <c r="L57" s="408"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -44023,22 +44059,22 @@
       <c r="C59" s="128">
         <v>44710</v>
       </c>
-      <c r="D59" s="373" t="s">
+      <c r="D59" s="384" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="374"/>
+      <c r="E59" s="385"/>
       <c r="F59" s="129">
         <v>149938.81</v>
       </c>
-      <c r="I59" s="375" t="s">
+      <c r="I59" s="386" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="376"/>
-      <c r="K59" s="377">
+      <c r="J59" s="387"/>
+      <c r="K59" s="388">
         <f>K55+K57</f>
         <v>-185321.84999999986</v>
       </c>
-      <c r="L59" s="377"/>
+      <c r="L59" s="388"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -44166,18 +44202,6 @@
     <sortCondition ref="J35:J40"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -44187,6 +44211,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 3 Nov 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #10  OCTUBRE 2022/BALANCE   HERRADURA  OCTUBRE      2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #10  OCTUBRE 2022/BALANCE   HERRADURA  OCTUBRE      2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="195" yWindow="915" windowWidth="16905" windowHeight="10110" firstSheet="17" activeTab="19"/>
+    <workbookView xWindow="195" yWindow="915" windowWidth="16905" windowHeight="10110" firstSheet="17" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 2         " sheetId="1" r:id="rId1"/>
@@ -632,7 +632,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="547">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2280,6 +2280,12 @@
   </si>
   <si>
     <t>D-15247</t>
+  </si>
+  <si>
+    <t>D-15466</t>
+  </si>
+  <si>
+    <t>D-15532</t>
   </si>
 </sst>
 </file>
@@ -3632,7 +3638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="415">
+  <cellXfs count="418">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -4320,38 +4326,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="44" fontId="3" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="44" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4434,6 +4411,39 @@
     <xf numFmtId="44" fontId="13" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4446,10 +4456,11 @@
     <xf numFmtId="166" fontId="12" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -9030,23 +9041,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -9056,21 +9067,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -9085,14 +9096,14 @@
       <c r="D4" s="16">
         <v>44563</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -9102,11 +9113,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -10561,11 +10572,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="391">
+      <c r="M40" s="382">
         <f>SUM(M5:M39)</f>
         <v>1527030</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>50013</v>
       </c>
@@ -10590,8 +10601,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="74"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -10798,29 +10809,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="395" t="s">
+      <c r="H53" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="396"/>
+      <c r="I53" s="387"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="397">
+      <c r="K53" s="388">
         <f>I51+L51</f>
         <v>50143.28</v>
       </c>
-      <c r="L53" s="398"/>
-      <c r="M53" s="399">
+      <c r="L53" s="389"/>
+      <c r="M53" s="390">
         <f>N40+M40</f>
         <v>1577043</v>
       </c>
-      <c r="N53" s="400"/>
+      <c r="N53" s="391"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="401" t="s">
+      <c r="D54" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="401"/>
+      <c r="E54" s="392"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>1561421.72</v>
@@ -10831,22 +10842,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="402" t="s">
+      <c r="D55" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="402"/>
+      <c r="E55" s="393"/>
       <c r="F55" s="111">
         <v>-1419082.77</v>
       </c>
-      <c r="I55" s="403" t="s">
+      <c r="I55" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="404"/>
-      <c r="K55" s="405">
+      <c r="J55" s="395"/>
+      <c r="K55" s="396">
         <f>F57+F58+F59</f>
         <v>296963.46999999997</v>
       </c>
-      <c r="L55" s="406"/>
+      <c r="L55" s="397"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -10877,11 +10888,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="407">
+      <c r="K57" s="398">
         <f>-C4</f>
         <v>-221059.7</v>
       </c>
-      <c r="L57" s="408"/>
+      <c r="L57" s="399"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -10898,22 +10909,22 @@
       <c r="C59" s="128">
         <v>44591</v>
       </c>
-      <c r="D59" s="384" t="s">
+      <c r="D59" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="385"/>
+      <c r="E59" s="376"/>
       <c r="F59" s="129">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="386" t="s">
+      <c r="I59" s="377" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="387"/>
-      <c r="K59" s="388">
+      <c r="J59" s="378"/>
+      <c r="K59" s="379">
         <f>K55+K57</f>
         <v>75903.76999999996</v>
       </c>
-      <c r="L59" s="388"/>
+      <c r="L59" s="379"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -11038,6 +11049,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
@@ -11053,12 +11070,6 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12511,23 +12522,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -12537,21 +12548,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -12566,14 +12577,14 @@
       <c r="D4" s="16">
         <v>44710</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -12583,11 +12594,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -14117,11 +14128,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="391">
+      <c r="M40" s="382">
         <f>SUM(M5:M39)</f>
         <v>2772689</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>107354</v>
       </c>
@@ -14152,8 +14163,8 @@
       <c r="L41" s="73">
         <v>638.99</v>
       </c>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -14399,29 +14410,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="395" t="s">
+      <c r="H53" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="396"/>
+      <c r="I53" s="387"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="397">
+      <c r="K53" s="388">
         <f>I51+L51</f>
         <v>60691.69</v>
       </c>
-      <c r="L53" s="398"/>
-      <c r="M53" s="399">
+      <c r="L53" s="389"/>
+      <c r="M53" s="390">
         <f>N40+M40</f>
         <v>2880043</v>
       </c>
-      <c r="N53" s="400"/>
+      <c r="N53" s="391"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="401" t="s">
+      <c r="D54" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="401"/>
+      <c r="E54" s="392"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2844548.31</v>
@@ -14432,22 +14443,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="402" t="s">
+      <c r="D55" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="402"/>
+      <c r="E55" s="393"/>
       <c r="F55" s="111">
         <v>-2875380.48</v>
       </c>
-      <c r="I55" s="403" t="s">
+      <c r="I55" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="404"/>
-      <c r="K55" s="405">
+      <c r="J55" s="395"/>
+      <c r="K55" s="396">
         <f>F57+F58+F59</f>
         <v>247554.74000000008</v>
       </c>
-      <c r="L55" s="406"/>
+      <c r="L55" s="397"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -14478,11 +14489,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="407">
+      <c r="K57" s="398">
         <f>-C4</f>
         <v>-149938.81</v>
       </c>
-      <c r="L57" s="408"/>
+      <c r="L57" s="399"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -14499,22 +14510,22 @@
       <c r="C59" s="128">
         <v>44745</v>
       </c>
-      <c r="D59" s="384" t="s">
+      <c r="D59" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="385"/>
+      <c r="E59" s="376"/>
       <c r="F59" s="129">
         <v>232165.91</v>
       </c>
-      <c r="I59" s="386" t="s">
+      <c r="I59" s="377" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="387"/>
-      <c r="K59" s="388">
+      <c r="J59" s="378"/>
+      <c r="K59" s="379">
         <f>K55+K57</f>
         <v>97615.93000000008</v>
       </c>
-      <c r="L59" s="388"/>
+      <c r="L59" s="379"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -14642,18 +14653,6 @@
     <sortCondition ref="B7:B9"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -14663,6 +14662,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.38" right="0.17" top="0.4" bottom="0.34" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -16144,23 +16155,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -16170,21 +16181,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -16199,14 +16210,14 @@
       <c r="D4" s="16">
         <v>44745</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -16216,11 +16227,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -17665,11 +17676,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="391">
+      <c r="M40" s="382">
         <f>SUM(M5:M39)</f>
         <v>2373103</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>67308</v>
       </c>
@@ -17698,8 +17709,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -17914,29 +17925,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="395" t="s">
+      <c r="H53" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="396"/>
+      <c r="I53" s="387"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="397">
+      <c r="K53" s="388">
         <f>I51+L51</f>
         <v>79649.720000000016</v>
       </c>
-      <c r="L53" s="398"/>
-      <c r="M53" s="399">
+      <c r="L53" s="389"/>
+      <c r="M53" s="390">
         <f>N40+M40</f>
         <v>2440411</v>
       </c>
-      <c r="N53" s="400"/>
+      <c r="N53" s="391"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="401" t="s">
+      <c r="D54" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="401"/>
+      <c r="E54" s="392"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2356249.2799999998</v>
@@ -17947,22 +17958,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="402" t="s">
+      <c r="D55" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="402"/>
+      <c r="E55" s="393"/>
       <c r="F55" s="111">
         <v>-2471332.31</v>
       </c>
-      <c r="I55" s="403" t="s">
+      <c r="I55" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="404"/>
-      <c r="K55" s="405">
+      <c r="J55" s="395"/>
+      <c r="K55" s="396">
         <f>F57+F58+F59</f>
         <v>214026.38999999972</v>
       </c>
-      <c r="L55" s="406"/>
+      <c r="L55" s="397"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -17993,11 +18004,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="407">
+      <c r="K57" s="398">
         <f>-C4</f>
         <v>-232165.91</v>
       </c>
-      <c r="L57" s="408"/>
+      <c r="L57" s="399"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -18014,22 +18025,22 @@
       <c r="C59" s="128">
         <v>44773</v>
       </c>
-      <c r="D59" s="384" t="s">
+      <c r="D59" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="385"/>
+      <c r="E59" s="376"/>
       <c r="F59" s="129">
         <v>273736.42</v>
       </c>
-      <c r="I59" s="386" t="s">
+      <c r="I59" s="377" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="387"/>
-      <c r="K59" s="388">
+      <c r="J59" s="378"/>
+      <c r="K59" s="379">
         <f>K55+K57</f>
         <v>-18139.520000000281</v>
       </c>
-      <c r="L59" s="388"/>
+      <c r="L59" s="379"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -18154,18 +18165,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -18175,6 +18174,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.27559055118110237" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="60" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19566,23 +19577,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>421</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -19592,21 +19603,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -19621,14 +19632,14 @@
       <c r="D4" s="16">
         <v>44773</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -19638,11 +19649,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -21122,11 +21133,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="391">
+      <c r="M40" s="382">
         <f>SUM(M5:M39)</f>
         <v>2375259</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>61117</v>
       </c>
@@ -21155,8 +21166,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -21371,29 +21382,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="395" t="s">
+      <c r="H53" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="396"/>
+      <c r="I53" s="387"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="397">
+      <c r="K53" s="388">
         <f>I51+L51</f>
         <v>52857.25</v>
       </c>
-      <c r="L53" s="398"/>
-      <c r="M53" s="399">
+      <c r="L53" s="389"/>
+      <c r="M53" s="390">
         <f>N40+M40</f>
         <v>2436376</v>
       </c>
-      <c r="N53" s="400"/>
+      <c r="N53" s="391"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="401" t="s">
+      <c r="D54" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="401"/>
+      <c r="E54" s="392"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2370653.75</v>
@@ -21404,22 +21415,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="402" t="s">
+      <c r="D55" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="402"/>
+      <c r="E55" s="393"/>
       <c r="F55" s="111">
         <v>-2401197.5699999998</v>
       </c>
-      <c r="I55" s="403" t="s">
+      <c r="I55" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="404"/>
-      <c r="K55" s="405">
+      <c r="J55" s="395"/>
+      <c r="K55" s="396">
         <f>F57+F58+F59</f>
         <v>259241.77000000016</v>
       </c>
-      <c r="L55" s="406"/>
+      <c r="L55" s="397"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -21450,11 +21461,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="407">
+      <c r="K57" s="398">
         <f>-C4</f>
         <v>-273736.42</v>
       </c>
-      <c r="L57" s="408"/>
+      <c r="L57" s="399"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -21471,22 +21482,22 @@
       <c r="C59" s="128">
         <v>44801</v>
       </c>
-      <c r="D59" s="384" t="s">
+      <c r="D59" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="385"/>
+      <c r="E59" s="376"/>
       <c r="F59" s="129">
         <v>236400.59</v>
       </c>
-      <c r="I59" s="410" t="s">
+      <c r="I59" s="412" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="411"/>
-      <c r="K59" s="412">
+      <c r="J59" s="413"/>
+      <c r="K59" s="414">
         <f>K55+K57</f>
         <v>-14494.64999999982</v>
       </c>
-      <c r="L59" s="412"/>
+      <c r="L59" s="414"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -21611,18 +21622,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -21632,6 +21631,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -23038,23 +23049,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>465</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -23064,21 +23075,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -23093,14 +23104,14 @@
       <c r="D4" s="16">
         <v>44801</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -23110,11 +23121,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -24842,11 +24853,11 @@
       <c r="L40" s="73">
         <v>927.48</v>
       </c>
-      <c r="M40" s="391">
+      <c r="M40" s="382">
         <f>SUM(M5:M39)</f>
         <v>3147309.5</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>76569</v>
       </c>
@@ -24881,8 +24892,8 @@
       <c r="L41" s="73">
         <v>33312</v>
       </c>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -25125,29 +25136,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="395" t="s">
+      <c r="H53" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="396"/>
+      <c r="I53" s="387"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="397">
+      <c r="K53" s="388">
         <f>I51+L51</f>
         <v>102873.87000000001</v>
       </c>
-      <c r="L53" s="398"/>
-      <c r="M53" s="399">
+      <c r="L53" s="389"/>
+      <c r="M53" s="390">
         <f>N40+M40</f>
         <v>3223878.5</v>
       </c>
-      <c r="N53" s="400"/>
+      <c r="N53" s="391"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="401" t="s">
+      <c r="D54" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="401"/>
+      <c r="E54" s="392"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>3130076.13</v>
@@ -25158,22 +25169,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="402" t="s">
+      <c r="D55" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="402"/>
+      <c r="E55" s="393"/>
       <c r="F55" s="111">
         <v>-3171951.31</v>
       </c>
-      <c r="I55" s="403" t="s">
+      <c r="I55" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="404"/>
-      <c r="K55" s="405">
+      <c r="J55" s="395"/>
+      <c r="K55" s="396">
         <f>F57+F58+F59</f>
         <v>265314.0299999998</v>
       </c>
-      <c r="L55" s="406"/>
+      <c r="L55" s="397"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -25204,11 +25215,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="407">
+      <c r="K57" s="398">
         <f>-C4</f>
         <v>-236400.59</v>
       </c>
-      <c r="L57" s="408"/>
+      <c r="L57" s="399"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -25225,22 +25236,22 @@
       <c r="C59" s="128">
         <v>44836</v>
       </c>
-      <c r="D59" s="384" t="s">
+      <c r="D59" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="385"/>
+      <c r="E59" s="376"/>
       <c r="F59" s="129">
         <v>242354.21</v>
       </c>
-      <c r="I59" s="410" t="s">
+      <c r="I59" s="412" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="411"/>
-      <c r="K59" s="412">
+      <c r="J59" s="413"/>
+      <c r="K59" s="414">
         <f>K55+K57</f>
         <v>28913.439999999799</v>
       </c>
-      <c r="L59" s="412"/>
+      <c r="L59" s="414"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -25368,6 +25379,18 @@
     <sortCondition ref="J41:J45"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -25377,18 +25400,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -26704,11 +26715,11 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C60" sqref="C60"/>
+      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26733,23 +26744,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>512</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -26759,21 +26770,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -26788,14 +26799,14 @@
       <c r="D4" s="16">
         <v>44836</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -26805,11 +26816,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -26898,7 +26909,7 @@
         <f>N6+M6+L6+I6+C6</f>
         <v>76332</v>
       </c>
-      <c r="Q6" s="413">
+      <c r="Q6" s="371">
         <v>0</v>
       </c>
       <c r="R6" s="283">
@@ -28452,11 +28463,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="360"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="391">
+      <c r="M40" s="382">
         <f>SUM(M5:M39)</f>
         <v>2563550</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>77235</v>
       </c>
@@ -28486,8 +28497,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="363"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -28702,29 +28713,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="395" t="s">
+      <c r="H53" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="396"/>
+      <c r="I53" s="387"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="397">
+      <c r="K53" s="388">
         <f>I51+L51</f>
         <v>43603</v>
       </c>
-      <c r="L53" s="398"/>
-      <c r="M53" s="399">
+      <c r="L53" s="389"/>
+      <c r="M53" s="390">
         <f>N40+M40</f>
         <v>2640785</v>
       </c>
-      <c r="N53" s="400"/>
+      <c r="N53" s="391"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="401" t="s">
+      <c r="D54" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="401"/>
+      <c r="E54" s="392"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2576003.7999999998</v>
@@ -28735,28 +28746,28 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="402" t="s">
+      <c r="D55" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="402"/>
+      <c r="E55" s="393"/>
       <c r="F55" s="111">
-        <v>0</v>
-      </c>
-      <c r="I55" s="403" t="s">
+        <v>-2793202.57</v>
+      </c>
+      <c r="I55" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="404"/>
-      <c r="K55" s="405">
+      <c r="J55" s="395"/>
+      <c r="K55" s="396">
         <f>F57+F58+F59</f>
-        <v>3050954.5599999996</v>
-      </c>
-      <c r="L55" s="406"/>
+        <v>257751.99</v>
+      </c>
+      <c r="L55" s="397"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D56" s="118"/>
-      <c r="E56" s="33"/>
+      <c r="E56" s="417"/>
       <c r="F56" s="119">
         <v>0</v>
       </c>
@@ -28774,18 +28785,18 @@
       </c>
       <c r="F57" s="111">
         <f>SUM(F54:F56)</f>
-        <v>2576003.7999999998</v>
+        <v>-217198.77000000002</v>
       </c>
       <c r="H57" s="22"/>
       <c r="I57" s="124" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="407">
+      <c r="K57" s="398">
         <f>-C4</f>
         <v>-242354.21</v>
       </c>
-      <c r="L57" s="408"/>
+      <c r="L57" s="399"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -28802,22 +28813,22 @@
       <c r="C59" s="128">
         <v>44864</v>
       </c>
-      <c r="D59" s="384" t="s">
+      <c r="D59" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="385"/>
+      <c r="E59" s="376"/>
       <c r="F59" s="129">
         <v>419424.76</v>
       </c>
-      <c r="I59" s="410" t="s">
+      <c r="I59" s="412" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="411"/>
-      <c r="K59" s="412">
+      <c r="J59" s="413"/>
+      <c r="K59" s="414">
         <f>K55+K57</f>
-        <v>2808600.3499999996</v>
-      </c>
-      <c r="L59" s="412"/>
+        <v>15397.779999999999</v>
+      </c>
+      <c r="L59" s="414"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -28942,18 +28953,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -28963,6 +28962,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30756,9 +30767,9 @@
   </sheetPr>
   <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30810,7 +30821,7 @@
       <c r="A3" s="254">
         <v>44837</v>
       </c>
-      <c r="B3" s="414" t="s">
+      <c r="B3" s="372" t="s">
         <v>520</v>
       </c>
       <c r="C3" s="256">
@@ -31170,13 +31181,13 @@
         <v>540</v>
       </c>
       <c r="C23" s="127">
-        <v>662896.04</v>
+        <v>66286.039999999994</v>
       </c>
       <c r="D23" s="304"/>
       <c r="E23" s="274"/>
       <c r="F23" s="188">
         <f t="shared" si="0"/>
-        <v>2478302.21</v>
+        <v>1881692.2099999997</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -31193,7 +31204,7 @@
       <c r="E24" s="274"/>
       <c r="F24" s="188">
         <f t="shared" si="0"/>
-        <v>2638055.23</v>
+        <v>2041445.2299999997</v>
       </c>
       <c r="G24" s="156"/>
     </row>
@@ -31211,7 +31222,7 @@
       <c r="E25" s="274"/>
       <c r="F25" s="188">
         <f t="shared" si="0"/>
-        <v>2774814.41</v>
+        <v>2178204.4099999997</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -31228,7 +31239,7 @@
       <c r="E26" s="127"/>
       <c r="F26" s="188">
         <f t="shared" si="0"/>
-        <v>2898754.39</v>
+        <v>2302144.3899999997</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -31245,29 +31256,41 @@
       <c r="E27" s="127"/>
       <c r="F27" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2465022.59</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="257"/>
-      <c r="B28" s="258"/>
-      <c r="C28" s="127"/>
+      <c r="A28" s="257">
+        <v>44863</v>
+      </c>
+      <c r="B28" s="415" t="s">
+        <v>545</v>
+      </c>
+      <c r="C28" s="416">
+        <v>174485.08</v>
+      </c>
       <c r="D28" s="259"/>
       <c r="E28" s="127"/>
       <c r="F28" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2639507.67</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="257"/>
-      <c r="B29" s="258"/>
-      <c r="C29" s="127"/>
+      <c r="A29" s="257">
+        <v>44864</v>
+      </c>
+      <c r="B29" s="415" t="s">
+        <v>546</v>
+      </c>
+      <c r="C29" s="416">
+        <v>153694.9</v>
+      </c>
       <c r="D29" s="259"/>
       <c r="E29" s="127"/>
       <c r="F29" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -31278,7 +31301,7 @@
       <c r="E30" s="127"/>
       <c r="F30" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -31289,7 +31312,7 @@
       <c r="E31" s="127"/>
       <c r="F31" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -31300,7 +31323,7 @@
       <c r="E32" s="127"/>
       <c r="F32" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
       <c r="G32" s="156"/>
     </row>
@@ -31312,7 +31335,7 @@
       <c r="E33" s="127"/>
       <c r="F33" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -31323,7 +31346,7 @@
       <c r="E34" s="127"/>
       <c r="F34" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -31334,7 +31357,7 @@
       <c r="E35" s="127"/>
       <c r="F35" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -31345,7 +31368,7 @@
       <c r="E36" s="127"/>
       <c r="F36" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -31356,7 +31379,7 @@
       <c r="E37" s="127"/>
       <c r="F37" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -31367,7 +31390,7 @@
       <c r="E38" s="127"/>
       <c r="F38" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -31378,7 +31401,7 @@
       <c r="E39" s="127"/>
       <c r="F39" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -31389,7 +31412,7 @@
       <c r="E40" s="84"/>
       <c r="F40" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -31400,7 +31423,7 @@
       <c r="E41" s="84"/>
       <c r="F41" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -31411,7 +31434,7 @@
       <c r="E42" s="84"/>
       <c r="F42" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -31422,7 +31445,7 @@
       <c r="E43" s="84"/>
       <c r="F43" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -31433,7 +31456,7 @@
       <c r="E44" s="84"/>
       <c r="F44" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31444,7 +31467,7 @@
       <c r="E45" s="84"/>
       <c r="F45" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31455,7 +31478,7 @@
       <c r="E46" s="84"/>
       <c r="F46" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31466,7 +31489,7 @@
       <c r="E47" s="84"/>
       <c r="F47" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31477,7 +31500,7 @@
       <c r="E48" s="84"/>
       <c r="F48" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31488,7 +31511,7 @@
       <c r="E49" s="84"/>
       <c r="F49" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31499,7 +31522,7 @@
       <c r="E50" s="84"/>
       <c r="F50" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31510,7 +31533,7 @@
       <c r="E51" s="84"/>
       <c r="F51" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31521,7 +31544,7 @@
       <c r="E52" s="84"/>
       <c r="F52" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31532,7 +31555,7 @@
       <c r="E53" s="84"/>
       <c r="F53" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31543,7 +31566,7 @@
       <c r="E54" s="84"/>
       <c r="F54" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31554,7 +31577,7 @@
       <c r="E55" s="84"/>
       <c r="F55" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31565,7 +31588,7 @@
       <c r="E56" s="84"/>
       <c r="F56" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31576,7 +31599,7 @@
       <c r="E57" s="84"/>
       <c r="F57" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31587,7 +31610,7 @@
       <c r="E58" s="84"/>
       <c r="F58" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31598,7 +31621,7 @@
       <c r="E59" s="84"/>
       <c r="F59" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31609,7 +31632,7 @@
       <c r="E60" s="84"/>
       <c r="F60" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31620,7 +31643,7 @@
       <c r="E61" s="84"/>
       <c r="F61" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31631,7 +31654,7 @@
       <c r="E62" s="32"/>
       <c r="F62" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31642,7 +31665,7 @@
       <c r="E63" s="32"/>
       <c r="F63" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31653,7 +31676,7 @@
       <c r="E64" s="32"/>
       <c r="F64" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31664,7 +31687,7 @@
       <c r="E65" s="32"/>
       <c r="F65" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31675,7 +31698,7 @@
       <c r="E66" s="32"/>
       <c r="F66" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31686,7 +31709,7 @@
       <c r="E67" s="32"/>
       <c r="F67" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31697,7 +31720,7 @@
       <c r="E68" s="84"/>
       <c r="F68" s="188">
         <f t="shared" si="0"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31708,7 +31731,7 @@
       <c r="E69" s="84"/>
       <c r="F69" s="188">
         <f t="shared" ref="F69:F78" si="1">C69-E69+F68</f>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31719,7 +31742,7 @@
       <c r="E70" s="84"/>
       <c r="F70" s="188">
         <f t="shared" si="1"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31730,7 +31753,7 @@
       <c r="E71" s="84"/>
       <c r="F71" s="188">
         <f t="shared" si="1"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31741,7 +31764,7 @@
       <c r="E72" s="84"/>
       <c r="F72" s="188">
         <f t="shared" si="1"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31752,7 +31775,7 @@
       <c r="E73" s="84"/>
       <c r="F73" s="188">
         <f t="shared" si="1"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31763,7 +31786,7 @@
       <c r="E74" s="84"/>
       <c r="F74" s="188">
         <f t="shared" si="1"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31774,7 +31797,7 @@
       <c r="E75" s="84"/>
       <c r="F75" s="188">
         <f t="shared" si="1"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31785,7 +31808,7 @@
       <c r="E76" s="84"/>
       <c r="F76" s="188">
         <f t="shared" si="1"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31796,7 +31819,7 @@
       <c r="E77" s="84"/>
       <c r="F77" s="188">
         <f t="shared" si="1"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31809,7 +31832,7 @@
       <c r="E78" s="32"/>
       <c r="F78" s="188">
         <f t="shared" si="1"/>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -31817,7 +31840,7 @@
       <c r="B79" s="223"/>
       <c r="C79" s="240">
         <f>SUM(C3:C78)</f>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
       <c r="D79" s="181"/>
       <c r="E79" s="170">
@@ -31826,7 +31849,7 @@
       </c>
       <c r="F79" s="171">
         <f>F78</f>
-        <v>3061632.5900000003</v>
+        <v>2793202.57</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -32015,23 +32038,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -32041,21 +32064,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -32070,14 +32093,14 @@
       <c r="D4" s="16">
         <v>44591</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -32087,11 +32110,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -33528,11 +33551,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="78"/>
-      <c r="M40" s="409">
+      <c r="M40" s="411">
         <f>SUM(M5:M39)</f>
         <v>1636108</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>55675</v>
       </c>
@@ -33557,8 +33580,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="74"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -33765,29 +33788,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="395" t="s">
+      <c r="H53" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="396"/>
+      <c r="I53" s="387"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="397">
+      <c r="K53" s="388">
         <f>I51+L51</f>
         <v>45634.280000000006</v>
       </c>
-      <c r="L53" s="398"/>
-      <c r="M53" s="399">
+      <c r="L53" s="389"/>
+      <c r="M53" s="390">
         <f>N40+M40</f>
         <v>1691783</v>
       </c>
-      <c r="N53" s="400"/>
+      <c r="N53" s="391"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="401" t="s">
+      <c r="D54" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="401"/>
+      <c r="E54" s="392"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>1686442.72</v>
@@ -33798,22 +33821,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="402" t="s">
+      <c r="D55" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="402"/>
+      <c r="E55" s="393"/>
       <c r="F55" s="111">
         <v>-1631962.77</v>
       </c>
-      <c r="I55" s="403" t="s">
+      <c r="I55" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="404"/>
-      <c r="K55" s="405">
+      <c r="J55" s="395"/>
+      <c r="K55" s="396">
         <f>F57+F58+F59</f>
         <v>238822.13999999996</v>
       </c>
-      <c r="L55" s="406"/>
+      <c r="L55" s="397"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -33844,11 +33867,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="407">
+      <c r="K57" s="398">
         <f>-C4</f>
         <v>-154314.51999999999</v>
       </c>
-      <c r="L57" s="408"/>
+      <c r="L57" s="399"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -33865,22 +33888,22 @@
       <c r="C59" s="128">
         <v>44619</v>
       </c>
-      <c r="D59" s="384" t="s">
+      <c r="D59" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="385"/>
+      <c r="E59" s="376"/>
       <c r="F59" s="129">
         <v>184342.19</v>
       </c>
-      <c r="I59" s="386" t="s">
+      <c r="I59" s="377" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="387"/>
-      <c r="K59" s="388">
+      <c r="J59" s="378"/>
+      <c r="K59" s="379">
         <f>K55+K57</f>
         <v>84507.619999999966</v>
       </c>
-      <c r="L59" s="388"/>
+      <c r="L59" s="379"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -34005,6 +34028,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -34014,18 +34049,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -35330,23 +35353,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -35356,21 +35379,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -35385,14 +35408,14 @@
       <c r="D4" s="16">
         <v>44619</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -35402,11 +35425,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -36857,11 +36880,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="391">
+      <c r="M40" s="382">
         <f>SUM(M5:M39)</f>
         <v>1793435</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>63995</v>
       </c>
@@ -36886,8 +36909,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -37026,29 +37049,29 @@
       <c r="A49" s="33"/>
       <c r="B49" s="113"/>
       <c r="C49" s="1"/>
-      <c r="H49" s="395" t="s">
+      <c r="H49" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="396"/>
+      <c r="I49" s="387"/>
       <c r="J49" s="114"/>
-      <c r="K49" s="397">
+      <c r="K49" s="388">
         <f>I47+L47</f>
         <v>90434.03</v>
       </c>
-      <c r="L49" s="398"/>
-      <c r="M49" s="399">
+      <c r="L49" s="389"/>
+      <c r="M49" s="390">
         <f>N40+M40</f>
         <v>1857430</v>
       </c>
-      <c r="N49" s="400"/>
+      <c r="N49" s="391"/>
       <c r="P49" s="32"/>
       <c r="Q49" s="8"/>
     </row>
     <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D50" s="401" t="s">
+      <c r="D50" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="401"/>
+      <c r="E50" s="392"/>
       <c r="F50" s="115">
         <f>F47-K49-C47</f>
         <v>1824260.97</v>
@@ -37059,22 +37082,22 @@
       <c r="Q50" s="8"/>
     </row>
     <row r="51" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D51" s="402" t="s">
+      <c r="D51" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="402"/>
+      <c r="E51" s="393"/>
       <c r="F51" s="111">
         <v>-1848136.64</v>
       </c>
-      <c r="I51" s="403" t="s">
+      <c r="I51" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J51" s="404"/>
-      <c r="K51" s="405">
+      <c r="J51" s="395"/>
+      <c r="K51" s="396">
         <f>F53+F54+F55</f>
         <v>195541.70000000007</v>
       </c>
-      <c r="L51" s="406"/>
+      <c r="L51" s="397"/>
       <c r="P51" s="32"/>
       <c r="Q51" s="8"/>
     </row>
@@ -37105,11 +37128,11 @@
         <v>17</v>
       </c>
       <c r="J53" s="125"/>
-      <c r="K53" s="407">
+      <c r="K53" s="398">
         <f>-C4</f>
         <v>-184342.19</v>
       </c>
-      <c r="L53" s="408"/>
+      <c r="L53" s="399"/>
     </row>
     <row r="54" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="126" t="s">
@@ -37126,22 +37149,22 @@
       <c r="C55" s="128">
         <v>44647</v>
       </c>
-      <c r="D55" s="384" t="s">
+      <c r="D55" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="385"/>
+      <c r="E55" s="376"/>
       <c r="F55" s="129">
         <v>219417.37</v>
       </c>
-      <c r="I55" s="386" t="s">
+      <c r="I55" s="377" t="s">
         <v>226</v>
       </c>
-      <c r="J55" s="387"/>
-      <c r="K55" s="388">
+      <c r="J55" s="378"/>
+      <c r="K55" s="379">
         <f>K51+K53</f>
         <v>11199.510000000068</v>
       </c>
-      <c r="L55" s="388"/>
+      <c r="L55" s="379"/>
     </row>
     <row r="56" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C56" s="130"/>
@@ -37269,18 +37292,6 @@
     <sortCondition ref="J34:J38"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -37290,6 +37301,18 @@
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="K49:L49"/>
     <mergeCell ref="M49:N49"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -38764,23 +38787,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -38790,21 +38813,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -38819,14 +38842,14 @@
       <c r="D4" s="16">
         <v>44647</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -38836,11 +38859,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -40437,11 +40460,11 @@
         <f>927.48+128</f>
         <v>1055.48</v>
       </c>
-      <c r="M40" s="391">
+      <c r="M40" s="382">
         <f>SUM(M5:M39)</f>
         <v>2146671</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>68590</v>
       </c>
@@ -40472,8 +40495,8 @@
       <c r="L41" s="73">
         <v>1195.68</v>
       </c>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -40704,29 +40727,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="395" t="s">
+      <c r="H53" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="396"/>
+      <c r="I53" s="387"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="397">
+      <c r="K53" s="388">
         <f>I51+L51</f>
         <v>91272.77</v>
       </c>
-      <c r="L53" s="398"/>
-      <c r="M53" s="399">
+      <c r="L53" s="389"/>
+      <c r="M53" s="390">
         <f>N40+M40</f>
         <v>2215261</v>
       </c>
-      <c r="N53" s="400"/>
+      <c r="N53" s="391"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="401" t="s">
+      <c r="D54" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="401"/>
+      <c r="E54" s="392"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2179879.23</v>
@@ -40737,22 +40760,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="402" t="s">
+      <c r="D55" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="402"/>
+      <c r="E55" s="393"/>
       <c r="F55" s="111">
         <v>-2227493.48</v>
       </c>
-      <c r="I55" s="403" t="s">
+      <c r="I55" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="404"/>
-      <c r="K55" s="405">
+      <c r="J55" s="395"/>
+      <c r="K55" s="396">
         <f>F57+F58+F59</f>
         <v>261521.34000000003</v>
       </c>
-      <c r="L55" s="406"/>
+      <c r="L55" s="397"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -40783,11 +40806,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="407">
+      <c r="K57" s="398">
         <f>-C4</f>
         <v>-219417.37</v>
       </c>
-      <c r="L57" s="408"/>
+      <c r="L57" s="399"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -40804,22 +40827,22 @@
       <c r="C59" s="128">
         <v>44682</v>
       </c>
-      <c r="D59" s="384" t="s">
+      <c r="D59" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="385"/>
+      <c r="E59" s="376"/>
       <c r="F59" s="129">
         <v>297874.59000000003</v>
       </c>
-      <c r="I59" s="386" t="s">
+      <c r="I59" s="377" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="387"/>
-      <c r="K59" s="388">
+      <c r="J59" s="378"/>
+      <c r="K59" s="379">
         <f>K55+K57</f>
         <v>42103.97000000003</v>
       </c>
-      <c r="L59" s="388"/>
+      <c r="L59" s="379"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -40947,18 +40970,6 @@
     <sortCondition ref="J40:J44"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -40968,6 +40979,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -42471,23 +42494,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="371"/>
-      <c r="C1" s="373" t="s">
+      <c r="B1" s="400"/>
+      <c r="C1" s="402" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
+      <c r="L1" s="403"/>
+      <c r="M1" s="403"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="372"/>
+      <c r="B2" s="401"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -42497,21 +42520,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="375" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="376"/>
+      <c r="B3" s="404" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="405"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="377" t="s">
+      <c r="H3" s="406" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="377"/>
+      <c r="I3" s="406"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="382" t="s">
+      <c r="R3" s="373" t="s">
         <v>38</v>
       </c>
     </row>
@@ -42526,14 +42549,14 @@
       <c r="D4" s="16">
         <v>44682</v>
       </c>
-      <c r="E4" s="378" t="s">
+      <c r="E4" s="407" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="379"/>
-      <c r="H4" s="380" t="s">
+      <c r="F4" s="408"/>
+      <c r="H4" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="381"/>
+      <c r="I4" s="410"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -42543,11 +42566,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="389" t="s">
+      <c r="P4" s="380" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="390"/>
-      <c r="R4" s="383"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -44064,11 +44087,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="391">
+      <c r="M40" s="382">
         <f>SUM(M5:M39)</f>
         <v>2144215</v>
       </c>
-      <c r="N40" s="393">
+      <c r="N40" s="384">
         <f>SUM(N5:N39)</f>
         <v>62525</v>
       </c>
@@ -44093,8 +44116,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="392"/>
-      <c r="N41" s="394"/>
+      <c r="M41" s="383"/>
+      <c r="N41" s="385"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -44305,29 +44328,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="395" t="s">
+      <c r="H53" s="386" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="396"/>
+      <c r="I53" s="387"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="397">
+      <c r="K53" s="388">
         <f>I51+L51</f>
         <v>51231.42</v>
       </c>
-      <c r="L53" s="398"/>
-      <c r="M53" s="399">
+      <c r="L53" s="389"/>
+      <c r="M53" s="390">
         <f>N40+M40</f>
         <v>2206740</v>
       </c>
-      <c r="N53" s="400"/>
+      <c r="N53" s="391"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="401" t="s">
+      <c r="D54" s="392" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="401"/>
+      <c r="E54" s="392"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2189405.58</v>
@@ -44338,22 +44361,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="402" t="s">
+      <c r="D55" s="393" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="402"/>
+      <c r="E55" s="393"/>
       <c r="F55" s="111">
         <v>-2251924.65</v>
       </c>
-      <c r="I55" s="403" t="s">
+      <c r="I55" s="394" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="404"/>
-      <c r="K55" s="405">
+      <c r="J55" s="395"/>
+      <c r="K55" s="396">
         <f>F57+F58+F59</f>
         <v>112552.74000000017</v>
       </c>
-      <c r="L55" s="406"/>
+      <c r="L55" s="397"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -44384,11 +44407,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="407">
+      <c r="K57" s="398">
         <f>-C4</f>
         <v>-297874.59000000003</v>
       </c>
-      <c r="L57" s="408"/>
+      <c r="L57" s="399"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -44405,22 +44428,22 @@
       <c r="C59" s="128">
         <v>44710</v>
       </c>
-      <c r="D59" s="384" t="s">
+      <c r="D59" s="375" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="385"/>
+      <c r="E59" s="376"/>
       <c r="F59" s="129">
         <v>149938.81</v>
       </c>
-      <c r="I59" s="386" t="s">
+      <c r="I59" s="377" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="387"/>
-      <c r="K59" s="388">
+      <c r="J59" s="378"/>
+      <c r="K59" s="379">
         <f>K55+K57</f>
         <v>-185321.84999999986</v>
       </c>
-      <c r="L59" s="388"/>
+      <c r="L59" s="379"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -44548,6 +44571,18 @@
     <sortCondition ref="J35:J40"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -44557,18 +44592,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>